<commit_message>
Update SIQ with Customer Answers
Add a new column with customer answers and delete an empty row

Co-Authored-By: ayahamdyahmed <ayahamdyahmed@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/SIQ 1.2.xlsx
+++ b/SIQ 1.2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="102">
   <si>
     <t>ID</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>SIQ_18</t>
-  </si>
-  <si>
-    <t>SIQ_19</t>
   </si>
   <si>
     <t>Every 5 orders the user will get only one order free</t>
@@ -376,9 +373,6 @@
     </r>
   </si>
   <si>
-    <t>Why Field is empty ?</t>
-  </si>
-  <si>
     <t>It calculate how many orders you need to have to free order</t>
   </si>
   <si>
@@ -445,6 +439,21 @@
     <t>what if the user want to search 
 in the resulted restaurants ? Shall he exaclty 
 wirte the restaurant name of substring of it ?</t>
+  </si>
+  <si>
+    <t>29/4/2018</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Make it substring</t>
+  </si>
+  <si>
+    <t>Not-Approved / that feature will be displayed on user account page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add customer Answers and solutions , delete an empty row </t>
   </si>
 </sst>
 </file>
@@ -947,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -965,72 +974,86 @@
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="14">
         <v>0.1</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="34.5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="14">
         <v>0.1</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="14">
         <v>1.2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="14">
         <v>1.2</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1.2</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1040,11 +1063,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1076,7 @@
     <col min="2" max="2" width="9.28515625" style="1"/>
     <col min="3" max="3" width="60.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="53.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" style="1"/>
     <col min="7" max="7" width="23.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
@@ -1071,10 +1094,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1085,10 +1108,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>63</v>
+      <c r="E2" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1102,7 +1128,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1116,7 +1145,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1127,10 +1159,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>66</v>
+      <c r="E5" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1141,10 +1176,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1155,10 +1193,13 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1169,10 +1210,13 @@
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1183,10 +1227,13 @@
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1202,6 +1249,9 @@
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1211,10 +1261,13 @@
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1225,22 +1278,33 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1248,55 +1312,67 @@
         <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>87</v>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1304,13 +1380,16 @@
         <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -1321,21 +1400,10 @@
         <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1346,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -1363,16 +1431,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -1380,10 +1448,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1391,10 +1459,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="103.5" x14ac:dyDescent="0.25">
@@ -1402,7 +1470,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="86.25" x14ac:dyDescent="0.25">
@@ -1410,10 +1478,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
@@ -1421,10 +1489,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1432,7 +1500,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1445,7 +1513,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
@@ -1453,62 +1521,54 @@
         <v>21</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>